<commit_message>
added names to the chart on the tasks
</commit_message>
<xml_diff>
--- a/gantt_chart_lofthus.xlsx
+++ b/gantt_chart_lofthus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fda248c8888d899/git_repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianlarsen/OneDrive/git_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{E2F956EC-ABCC-644E-865C-E94541B67F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8518D39B-BF0F-0142-B107-D762BBF87E6E}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="8_{E2F956EC-ABCC-644E-865C-E94541B67F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C0B220D0-A6B8-9444-819D-0F406CCD3B5B}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="460" windowWidth="30200" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="153">
   <si>
     <t>Input Cell</t>
   </si>
@@ -1158,6 +1158,9 @@
   </si>
   <si>
     <t>10 Work days</t>
+  </si>
+  <si>
+    <t>Christian</t>
   </si>
 </sst>
 </file>
@@ -2059,7 +2062,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -2299,17 +2302,8 @@
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2344,20 +2338,12 @@
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="61" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="61" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -2405,25 +2391,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="62" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="62" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="62" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -2438,6 +2406,38 @@
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="61" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="61" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="62" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="62" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="62" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3217,7 +3217,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -3236,42 +3236,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="30" customHeight="1">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="143" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="155"/>
+      <c r="B1" s="144"/>
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
       <c r="I1" s="75"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="106"/>
-      <c r="R1" s="106"/>
-      <c r="S1" s="106"/>
-      <c r="T1" s="106"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-      <c r="X1" s="106"/>
-      <c r="Y1" s="106"/>
-      <c r="Z1" s="106"/>
-      <c r="AA1" s="106"/>
-      <c r="AB1" s="106"/>
-      <c r="AC1" s="106"/>
-      <c r="AD1" s="106"/>
-      <c r="AE1" s="106"/>
+      <c r="K1" s="145"/>
+      <c r="L1" s="145"/>
+      <c r="M1" s="145"/>
+      <c r="N1" s="145"/>
+      <c r="O1" s="145"/>
+      <c r="P1" s="145"/>
+      <c r="Q1" s="145"/>
+      <c r="R1" s="145"/>
+      <c r="S1" s="145"/>
+      <c r="T1" s="145"/>
+      <c r="U1" s="145"/>
+      <c r="V1" s="145"/>
+      <c r="W1" s="145"/>
+      <c r="X1" s="145"/>
+      <c r="Y1" s="145"/>
+      <c r="Z1" s="145"/>
+      <c r="AA1" s="145"/>
+      <c r="AB1" s="145"/>
+      <c r="AC1" s="145"/>
+      <c r="AD1" s="145"/>
+      <c r="AE1" s="145"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1">
-      <c r="A2" s="152" t="s">
+      <c r="A2" s="141" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="153"/>
+      <c r="B2" s="142"/>
       <c r="C2" s="22"/>
       <c r="D2" s="29"/>
       <c r="E2" s="103"/>
@@ -3287,264 +3287,264 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="143"/>
-      <c r="N3" s="143"/>
-      <c r="O3" s="143"/>
-      <c r="P3" s="143"/>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="143"/>
-      <c r="S3" s="143"/>
-      <c r="T3" s="143"/>
-      <c r="U3" s="143"/>
-      <c r="V3" s="143"/>
-      <c r="W3" s="143"/>
-      <c r="X3" s="143"/>
-      <c r="Y3" s="143"/>
-      <c r="Z3" s="143"/>
-      <c r="AA3" s="143"/>
-      <c r="AB3" s="142"/>
-      <c r="AC3" s="142"/>
-      <c r="AD3" s="142"/>
-      <c r="AE3" s="142"/>
-      <c r="AF3" s="142"/>
-      <c r="AG3" s="142"/>
-      <c r="AH3" s="142"/>
-      <c r="AI3" s="142"/>
-      <c r="AJ3" s="142"/>
-      <c r="AK3" s="142"/>
-      <c r="AL3" s="142"/>
-      <c r="AM3" s="142"/>
-      <c r="AN3" s="142"/>
-      <c r="AO3" s="142"/>
-      <c r="AP3" s="142"/>
-      <c r="AQ3" s="142"/>
-      <c r="AR3" s="142"/>
-      <c r="AS3" s="142"/>
-      <c r="AT3" s="142"/>
-      <c r="AU3" s="142"/>
-      <c r="AV3" s="142"/>
-      <c r="AW3" s="142"/>
-      <c r="AX3" s="142"/>
-      <c r="AY3" s="142"/>
-      <c r="AZ3" s="142"/>
-      <c r="BA3" s="142"/>
-      <c r="BB3" s="142"/>
-      <c r="BC3" s="142"/>
-      <c r="BD3" s="142"/>
-      <c r="BE3" s="142"/>
-      <c r="BF3" s="142"/>
-      <c r="BG3" s="142"/>
-      <c r="BH3" s="142"/>
-      <c r="BI3" s="142"/>
-      <c r="BJ3" s="142"/>
-      <c r="BK3" s="142"/>
-      <c r="BL3" s="142"/>
-      <c r="BM3" s="142"/>
-      <c r="BN3" s="142"/>
+      <c r="I3" s="136"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="138"/>
+      <c r="O3" s="138"/>
+      <c r="P3" s="138"/>
+      <c r="Q3" s="138"/>
+      <c r="R3" s="138"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="138"/>
+      <c r="U3" s="138"/>
+      <c r="V3" s="138"/>
+      <c r="W3" s="138"/>
+      <c r="X3" s="138"/>
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="138"/>
+      <c r="AA3" s="138"/>
+      <c r="AB3" s="137"/>
+      <c r="AC3" s="137"/>
+      <c r="AD3" s="137"/>
+      <c r="AE3" s="137"/>
+      <c r="AF3" s="137"/>
+      <c r="AG3" s="137"/>
+      <c r="AH3" s="137"/>
+      <c r="AI3" s="137"/>
+      <c r="AJ3" s="137"/>
+      <c r="AK3" s="137"/>
+      <c r="AL3" s="137"/>
+      <c r="AM3" s="137"/>
+      <c r="AN3" s="137"/>
+      <c r="AO3" s="137"/>
+      <c r="AP3" s="137"/>
+      <c r="AQ3" s="137"/>
+      <c r="AR3" s="137"/>
+      <c r="AS3" s="137"/>
+      <c r="AT3" s="137"/>
+      <c r="AU3" s="137"/>
+      <c r="AV3" s="137"/>
+      <c r="AW3" s="137"/>
+      <c r="AX3" s="137"/>
+      <c r="AY3" s="137"/>
+      <c r="AZ3" s="137"/>
+      <c r="BA3" s="137"/>
+      <c r="BB3" s="137"/>
+      <c r="BC3" s="137"/>
+      <c r="BD3" s="137"/>
+      <c r="BE3" s="137"/>
+      <c r="BF3" s="137"/>
+      <c r="BG3" s="137"/>
+      <c r="BH3" s="137"/>
+      <c r="BI3" s="137"/>
+      <c r="BJ3" s="137"/>
+      <c r="BK3" s="137"/>
+      <c r="BL3" s="137"/>
+      <c r="BM3" s="137"/>
+      <c r="BN3" s="137"/>
     </row>
     <row r="4" spans="1:66" ht="17.25" customHeight="1">
-      <c r="A4" s="120"/>
-      <c r="B4" s="127" t="s">
+      <c r="A4" s="117"/>
+      <c r="B4" s="122" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="122">
+      <c r="C4" s="150">
         <v>43129</v>
       </c>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="121" t="s">
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="124">
+      <c r="H4" s="120">
         <v>1</v>
       </c>
-      <c r="I4" s="144"/>
-      <c r="J4" s="142"/>
-      <c r="K4" s="145" t="str">
+      <c r="I4" s="139"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="147" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="146"/>
-      <c r="M4" s="146"/>
-      <c r="N4" s="146"/>
-      <c r="O4" s="146"/>
-      <c r="P4" s="146"/>
-      <c r="Q4" s="147"/>
-      <c r="R4" s="145" t="str">
+      <c r="L4" s="148"/>
+      <c r="M4" s="148"/>
+      <c r="N4" s="148"/>
+      <c r="O4" s="148"/>
+      <c r="P4" s="148"/>
+      <c r="Q4" s="149"/>
+      <c r="R4" s="147" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="146"/>
-      <c r="T4" s="146"/>
-      <c r="U4" s="146"/>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="147"/>
-      <c r="Y4" s="145" t="str">
+      <c r="S4" s="148"/>
+      <c r="T4" s="148"/>
+      <c r="U4" s="148"/>
+      <c r="V4" s="148"/>
+      <c r="W4" s="148"/>
+      <c r="X4" s="149"/>
+      <c r="Y4" s="147" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="146"/>
-      <c r="AA4" s="146"/>
-      <c r="AB4" s="146"/>
-      <c r="AC4" s="146"/>
-      <c r="AD4" s="146"/>
-      <c r="AE4" s="147"/>
-      <c r="AF4" s="145" t="str">
+      <c r="Z4" s="148"/>
+      <c r="AA4" s="148"/>
+      <c r="AB4" s="148"/>
+      <c r="AC4" s="148"/>
+      <c r="AD4" s="148"/>
+      <c r="AE4" s="149"/>
+      <c r="AF4" s="147" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="146"/>
-      <c r="AH4" s="146"/>
-      <c r="AI4" s="146"/>
-      <c r="AJ4" s="146"/>
-      <c r="AK4" s="146"/>
-      <c r="AL4" s="147"/>
-      <c r="AM4" s="145" t="str">
+      <c r="AG4" s="148"/>
+      <c r="AH4" s="148"/>
+      <c r="AI4" s="148"/>
+      <c r="AJ4" s="148"/>
+      <c r="AK4" s="148"/>
+      <c r="AL4" s="149"/>
+      <c r="AM4" s="147" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="146"/>
-      <c r="AO4" s="146"/>
-      <c r="AP4" s="146"/>
-      <c r="AQ4" s="146"/>
-      <c r="AR4" s="146"/>
-      <c r="AS4" s="147"/>
-      <c r="AT4" s="145" t="str">
+      <c r="AN4" s="148"/>
+      <c r="AO4" s="148"/>
+      <c r="AP4" s="148"/>
+      <c r="AQ4" s="148"/>
+      <c r="AR4" s="148"/>
+      <c r="AS4" s="149"/>
+      <c r="AT4" s="147" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="146"/>
-      <c r="AV4" s="146"/>
-      <c r="AW4" s="146"/>
-      <c r="AX4" s="146"/>
-      <c r="AY4" s="146"/>
-      <c r="AZ4" s="147"/>
-      <c r="BA4" s="145" t="str">
+      <c r="AU4" s="148"/>
+      <c r="AV4" s="148"/>
+      <c r="AW4" s="148"/>
+      <c r="AX4" s="148"/>
+      <c r="AY4" s="148"/>
+      <c r="AZ4" s="149"/>
+      <c r="BA4" s="147" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="146"/>
-      <c r="BC4" s="146"/>
-      <c r="BD4" s="146"/>
-      <c r="BE4" s="146"/>
-      <c r="BF4" s="146"/>
-      <c r="BG4" s="147"/>
-      <c r="BH4" s="145" t="str">
+      <c r="BB4" s="148"/>
+      <c r="BC4" s="148"/>
+      <c r="BD4" s="148"/>
+      <c r="BE4" s="148"/>
+      <c r="BF4" s="148"/>
+      <c r="BG4" s="149"/>
+      <c r="BH4" s="147" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="146"/>
-      <c r="BJ4" s="146"/>
-      <c r="BK4" s="146"/>
-      <c r="BL4" s="146"/>
-      <c r="BM4" s="146"/>
-      <c r="BN4" s="147"/>
+      <c r="BI4" s="148"/>
+      <c r="BJ4" s="148"/>
+      <c r="BK4" s="148"/>
+      <c r="BL4" s="148"/>
+      <c r="BM4" s="148"/>
+      <c r="BN4" s="149"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1">
-      <c r="A5" s="120"/>
-      <c r="B5" s="127" t="s">
+      <c r="A5" s="117"/>
+      <c r="B5" s="122" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="125" t="s">
+      <c r="C5" s="146" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="125"/>
-      <c r="E5" s="125"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="148"/>
-      <c r="J5" s="142"/>
-      <c r="K5" s="149">
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="140"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="151">
         <f>K6</f>
         <v>43129</v>
       </c>
-      <c r="L5" s="150"/>
-      <c r="M5" s="150"/>
-      <c r="N5" s="150"/>
-      <c r="O5" s="150"/>
-      <c r="P5" s="150"/>
-      <c r="Q5" s="151"/>
-      <c r="R5" s="149">
+      <c r="L5" s="152"/>
+      <c r="M5" s="152"/>
+      <c r="N5" s="152"/>
+      <c r="O5" s="152"/>
+      <c r="P5" s="152"/>
+      <c r="Q5" s="153"/>
+      <c r="R5" s="151">
         <f>R6</f>
         <v>43136</v>
       </c>
-      <c r="S5" s="150"/>
-      <c r="T5" s="150"/>
-      <c r="U5" s="150"/>
-      <c r="V5" s="150"/>
-      <c r="W5" s="150"/>
-      <c r="X5" s="151"/>
-      <c r="Y5" s="149">
+      <c r="S5" s="152"/>
+      <c r="T5" s="152"/>
+      <c r="U5" s="152"/>
+      <c r="V5" s="152"/>
+      <c r="W5" s="152"/>
+      <c r="X5" s="153"/>
+      <c r="Y5" s="151">
         <f>Y6</f>
         <v>43143</v>
       </c>
-      <c r="Z5" s="150"/>
-      <c r="AA5" s="150"/>
-      <c r="AB5" s="150"/>
-      <c r="AC5" s="150"/>
-      <c r="AD5" s="150"/>
-      <c r="AE5" s="151"/>
-      <c r="AF5" s="149">
+      <c r="Z5" s="152"/>
+      <c r="AA5" s="152"/>
+      <c r="AB5" s="152"/>
+      <c r="AC5" s="152"/>
+      <c r="AD5" s="152"/>
+      <c r="AE5" s="153"/>
+      <c r="AF5" s="151">
         <f>AF6</f>
         <v>43150</v>
       </c>
-      <c r="AG5" s="150"/>
-      <c r="AH5" s="150"/>
-      <c r="AI5" s="150"/>
-      <c r="AJ5" s="150"/>
-      <c r="AK5" s="150"/>
-      <c r="AL5" s="151"/>
-      <c r="AM5" s="149">
+      <c r="AG5" s="152"/>
+      <c r="AH5" s="152"/>
+      <c r="AI5" s="152"/>
+      <c r="AJ5" s="152"/>
+      <c r="AK5" s="152"/>
+      <c r="AL5" s="153"/>
+      <c r="AM5" s="151">
         <f>AM6</f>
         <v>43157</v>
       </c>
-      <c r="AN5" s="150"/>
-      <c r="AO5" s="150"/>
-      <c r="AP5" s="150"/>
-      <c r="AQ5" s="150"/>
-      <c r="AR5" s="150"/>
-      <c r="AS5" s="151"/>
-      <c r="AT5" s="149">
+      <c r="AN5" s="152"/>
+      <c r="AO5" s="152"/>
+      <c r="AP5" s="152"/>
+      <c r="AQ5" s="152"/>
+      <c r="AR5" s="152"/>
+      <c r="AS5" s="153"/>
+      <c r="AT5" s="151">
         <f>AT6</f>
         <v>43164</v>
       </c>
-      <c r="AU5" s="150"/>
-      <c r="AV5" s="150"/>
-      <c r="AW5" s="150"/>
-      <c r="AX5" s="150"/>
-      <c r="AY5" s="150"/>
-      <c r="AZ5" s="151"/>
-      <c r="BA5" s="149">
+      <c r="AU5" s="152"/>
+      <c r="AV5" s="152"/>
+      <c r="AW5" s="152"/>
+      <c r="AX5" s="152"/>
+      <c r="AY5" s="152"/>
+      <c r="AZ5" s="153"/>
+      <c r="BA5" s="151">
         <f>BA6</f>
         <v>43171</v>
       </c>
-      <c r="BB5" s="150"/>
-      <c r="BC5" s="150"/>
-      <c r="BD5" s="150"/>
-      <c r="BE5" s="150"/>
-      <c r="BF5" s="150"/>
-      <c r="BG5" s="151"/>
-      <c r="BH5" s="149">
+      <c r="BB5" s="152"/>
+      <c r="BC5" s="152"/>
+      <c r="BD5" s="152"/>
+      <c r="BE5" s="152"/>
+      <c r="BF5" s="152"/>
+      <c r="BG5" s="153"/>
+      <c r="BH5" s="151">
         <f>BH6</f>
         <v>43178</v>
       </c>
-      <c r="BI5" s="150"/>
-      <c r="BJ5" s="150"/>
-      <c r="BK5" s="150"/>
-      <c r="BL5" s="150"/>
-      <c r="BM5" s="150"/>
-      <c r="BN5" s="151"/>
+      <c r="BI5" s="152"/>
+      <c r="BJ5" s="152"/>
+      <c r="BK5" s="152"/>
+      <c r="BL5" s="152"/>
+      <c r="BM5" s="152"/>
+      <c r="BN5" s="153"/>
     </row>
     <row r="6" spans="1:66" ht="14">
       <c r="A6" s="44"/>
-      <c r="B6" s="128"/>
+      <c r="B6" s="123"/>
       <c r="C6" s="45"/>
       <c r="D6" s="46"/>
       <c r="E6" s="45"/>
@@ -3552,485 +3552,485 @@
       <c r="G6" s="45"/>
       <c r="H6" s="45"/>
       <c r="I6" s="45"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="134">
+      <c r="J6" s="121"/>
+      <c r="K6" s="129">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
         <v>43129</v>
       </c>
-      <c r="L6" s="135">
+      <c r="L6" s="130">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
         <v>43130</v>
       </c>
-      <c r="M6" s="135">
+      <c r="M6" s="130">
         <f t="shared" si="0"/>
         <v>43131</v>
       </c>
-      <c r="N6" s="135">
+      <c r="N6" s="130">
         <f t="shared" si="0"/>
         <v>43132</v>
       </c>
-      <c r="O6" s="135">
+      <c r="O6" s="130">
         <f t="shared" si="0"/>
         <v>43133</v>
       </c>
-      <c r="P6" s="135">
+      <c r="P6" s="130">
         <f t="shared" si="0"/>
         <v>43134</v>
       </c>
-      <c r="Q6" s="136">
+      <c r="Q6" s="131">
         <f t="shared" si="0"/>
         <v>43135</v>
       </c>
-      <c r="R6" s="134">
+      <c r="R6" s="129">
         <f t="shared" si="0"/>
         <v>43136</v>
       </c>
-      <c r="S6" s="135">
+      <c r="S6" s="130">
         <f t="shared" si="0"/>
         <v>43137</v>
       </c>
-      <c r="T6" s="135">
+      <c r="T6" s="130">
         <f t="shared" si="0"/>
         <v>43138</v>
       </c>
-      <c r="U6" s="135">
+      <c r="U6" s="130">
         <f t="shared" si="0"/>
         <v>43139</v>
       </c>
-      <c r="V6" s="135">
+      <c r="V6" s="130">
         <f t="shared" si="0"/>
         <v>43140</v>
       </c>
-      <c r="W6" s="135">
+      <c r="W6" s="130">
         <f t="shared" si="0"/>
         <v>43141</v>
       </c>
-      <c r="X6" s="136">
+      <c r="X6" s="131">
         <f t="shared" si="0"/>
         <v>43142</v>
       </c>
-      <c r="Y6" s="134">
+      <c r="Y6" s="129">
         <f t="shared" si="0"/>
         <v>43143</v>
       </c>
-      <c r="Z6" s="135">
+      <c r="Z6" s="130">
         <f t="shared" si="0"/>
         <v>43144</v>
       </c>
-      <c r="AA6" s="135">
+      <c r="AA6" s="130">
         <f t="shared" si="0"/>
         <v>43145</v>
       </c>
-      <c r="AB6" s="135">
+      <c r="AB6" s="130">
         <f t="shared" si="0"/>
         <v>43146</v>
       </c>
-      <c r="AC6" s="135">
+      <c r="AC6" s="130">
         <f t="shared" si="0"/>
         <v>43147</v>
       </c>
-      <c r="AD6" s="135">
+      <c r="AD6" s="130">
         <f t="shared" si="0"/>
         <v>43148</v>
       </c>
-      <c r="AE6" s="136">
+      <c r="AE6" s="131">
         <f t="shared" si="0"/>
         <v>43149</v>
       </c>
-      <c r="AF6" s="134">
+      <c r="AF6" s="129">
         <f t="shared" si="0"/>
         <v>43150</v>
       </c>
-      <c r="AG6" s="135">
+      <c r="AG6" s="130">
         <f t="shared" si="0"/>
         <v>43151</v>
       </c>
-      <c r="AH6" s="135">
+      <c r="AH6" s="130">
         <f t="shared" si="0"/>
         <v>43152</v>
       </c>
-      <c r="AI6" s="135">
+      <c r="AI6" s="130">
         <f t="shared" si="0"/>
         <v>43153</v>
       </c>
-      <c r="AJ6" s="135">
+      <c r="AJ6" s="130">
         <f t="shared" si="0"/>
         <v>43154</v>
       </c>
-      <c r="AK6" s="135">
+      <c r="AK6" s="130">
         <f t="shared" si="0"/>
         <v>43155</v>
       </c>
-      <c r="AL6" s="136">
+      <c r="AL6" s="131">
         <f t="shared" si="0"/>
         <v>43156</v>
       </c>
-      <c r="AM6" s="134">
+      <c r="AM6" s="129">
         <f t="shared" si="0"/>
         <v>43157</v>
       </c>
-      <c r="AN6" s="135">
+      <c r="AN6" s="130">
         <f t="shared" si="0"/>
         <v>43158</v>
       </c>
-      <c r="AO6" s="135">
+      <c r="AO6" s="130">
         <f t="shared" si="0"/>
         <v>43159</v>
       </c>
-      <c r="AP6" s="135">
+      <c r="AP6" s="130">
         <f t="shared" si="0"/>
         <v>43160</v>
       </c>
-      <c r="AQ6" s="135">
+      <c r="AQ6" s="130">
         <f t="shared" si="0"/>
         <v>43161</v>
       </c>
-      <c r="AR6" s="135">
+      <c r="AR6" s="130">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
         <v>43162</v>
       </c>
-      <c r="AS6" s="136">
+      <c r="AS6" s="131">
         <f t="shared" si="1"/>
         <v>43163</v>
       </c>
-      <c r="AT6" s="134">
+      <c r="AT6" s="129">
         <f t="shared" si="1"/>
         <v>43164</v>
       </c>
-      <c r="AU6" s="135">
+      <c r="AU6" s="130">
         <f t="shared" si="1"/>
         <v>43165</v>
       </c>
-      <c r="AV6" s="135">
+      <c r="AV6" s="130">
         <f t="shared" si="1"/>
         <v>43166</v>
       </c>
-      <c r="AW6" s="135">
+      <c r="AW6" s="130">
         <f t="shared" si="1"/>
         <v>43167</v>
       </c>
-      <c r="AX6" s="135">
+      <c r="AX6" s="130">
         <f t="shared" si="1"/>
         <v>43168</v>
       </c>
-      <c r="AY6" s="135">
+      <c r="AY6" s="130">
         <f t="shared" si="1"/>
         <v>43169</v>
       </c>
-      <c r="AZ6" s="136">
+      <c r="AZ6" s="131">
         <f t="shared" si="1"/>
         <v>43170</v>
       </c>
-      <c r="BA6" s="134">
+      <c r="BA6" s="129">
         <f t="shared" si="1"/>
         <v>43171</v>
       </c>
-      <c r="BB6" s="135">
+      <c r="BB6" s="130">
         <f t="shared" si="1"/>
         <v>43172</v>
       </c>
-      <c r="BC6" s="135">
+      <c r="BC6" s="130">
         <f t="shared" si="1"/>
         <v>43173</v>
       </c>
-      <c r="BD6" s="135">
+      <c r="BD6" s="130">
         <f t="shared" si="1"/>
         <v>43174</v>
       </c>
-      <c r="BE6" s="135">
+      <c r="BE6" s="130">
         <f t="shared" si="1"/>
         <v>43175</v>
       </c>
-      <c r="BF6" s="135">
+      <c r="BF6" s="130">
         <f t="shared" si="1"/>
         <v>43176</v>
       </c>
-      <c r="BG6" s="136">
+      <c r="BG6" s="131">
         <f t="shared" si="1"/>
         <v>43177</v>
       </c>
-      <c r="BH6" s="134">
+      <c r="BH6" s="129">
         <f t="shared" si="1"/>
         <v>43178</v>
       </c>
-      <c r="BI6" s="135">
+      <c r="BI6" s="130">
         <f t="shared" si="1"/>
         <v>43179</v>
       </c>
-      <c r="BJ6" s="135">
+      <c r="BJ6" s="130">
         <f t="shared" si="1"/>
         <v>43180</v>
       </c>
-      <c r="BK6" s="135">
+      <c r="BK6" s="130">
         <f t="shared" si="1"/>
         <v>43181</v>
       </c>
-      <c r="BL6" s="135">
+      <c r="BL6" s="130">
         <f t="shared" si="1"/>
         <v>43182</v>
       </c>
-      <c r="BM6" s="135">
+      <c r="BM6" s="130">
         <f t="shared" si="1"/>
         <v>43183</v>
       </c>
-      <c r="BN6" s="136">
+      <c r="BN6" s="131">
         <f t="shared" si="1"/>
         <v>43184</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="74" customFormat="1" ht="43" thickBot="1">
-      <c r="A7" s="129"/>
-      <c r="B7" s="130" t="s">
+      <c r="A7" s="124"/>
+      <c r="B7" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="131" t="s">
+      <c r="C7" s="126" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="132" t="s">
+      <c r="D7" s="127" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="133" t="s">
+      <c r="E7" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="133" t="s">
+      <c r="F7" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="131" t="s">
+      <c r="G7" s="126" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="131" t="s">
+      <c r="H7" s="126" t="s">
         <v>64</v>
       </c>
       <c r="I7" s="73"/>
-      <c r="J7" s="137"/>
-      <c r="K7" s="138" t="str">
+      <c r="J7" s="132"/>
+      <c r="K7" s="133" t="str">
         <f t="shared" ref="K7:AP7" si="2">CHOOSE(WEEKDAY(K6,1),"S","M","T","W","T","F","S")</f>
         <v>M</v>
       </c>
-      <c r="L7" s="139" t="str">
+      <c r="L7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="M7" s="139" t="str">
+      <c r="M7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>W</v>
       </c>
-      <c r="N7" s="139" t="str">
+      <c r="N7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="O7" s="139" t="str">
+      <c r="O7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="P7" s="139" t="str">
+      <c r="P7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="Q7" s="140" t="str">
+      <c r="Q7" s="135" t="str">
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="R7" s="138" t="str">
+      <c r="R7" s="133" t="str">
         <f t="shared" si="2"/>
         <v>M</v>
       </c>
-      <c r="S7" s="139" t="str">
+      <c r="S7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="T7" s="139" t="str">
+      <c r="T7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>W</v>
       </c>
-      <c r="U7" s="139" t="str">
+      <c r="U7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="V7" s="139" t="str">
+      <c r="V7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="W7" s="139" t="str">
+      <c r="W7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="X7" s="140" t="str">
+      <c r="X7" s="135" t="str">
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="Y7" s="138" t="str">
+      <c r="Y7" s="133" t="str">
         <f t="shared" si="2"/>
         <v>M</v>
       </c>
-      <c r="Z7" s="139" t="str">
+      <c r="Z7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="AA7" s="139" t="str">
+      <c r="AA7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>W</v>
       </c>
-      <c r="AB7" s="139" t="str">
+      <c r="AB7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="AC7" s="139" t="str">
+      <c r="AC7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="AD7" s="139" t="str">
+      <c r="AD7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="AE7" s="140" t="str">
+      <c r="AE7" s="135" t="str">
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="AF7" s="138" t="str">
+      <c r="AF7" s="133" t="str">
         <f t="shared" si="2"/>
         <v>M</v>
       </c>
-      <c r="AG7" s="139" t="str">
+      <c r="AG7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="AH7" s="139" t="str">
+      <c r="AH7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>W</v>
       </c>
-      <c r="AI7" s="139" t="str">
+      <c r="AI7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="AJ7" s="139" t="str">
+      <c r="AJ7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>F</v>
       </c>
-      <c r="AK7" s="139" t="str">
+      <c r="AK7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="AL7" s="140" t="str">
+      <c r="AL7" s="135" t="str">
         <f t="shared" si="2"/>
         <v>S</v>
       </c>
-      <c r="AM7" s="138" t="str">
+      <c r="AM7" s="133" t="str">
         <f t="shared" si="2"/>
         <v>M</v>
       </c>
-      <c r="AN7" s="139" t="str">
+      <c r="AN7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="AO7" s="139" t="str">
+      <c r="AO7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>W</v>
       </c>
-      <c r="AP7" s="139" t="str">
+      <c r="AP7" s="134" t="str">
         <f t="shared" si="2"/>
         <v>T</v>
       </c>
-      <c r="AQ7" s="139" t="str">
+      <c r="AQ7" s="134" t="str">
         <f t="shared" ref="AQ7:BN7" si="3">CHOOSE(WEEKDAY(AQ6,1),"S","M","T","W","T","F","S")</f>
         <v>F</v>
       </c>
-      <c r="AR7" s="139" t="str">
+      <c r="AR7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="AS7" s="140" t="str">
+      <c r="AS7" s="135" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="AT7" s="138" t="str">
+      <c r="AT7" s="133" t="str">
         <f t="shared" si="3"/>
         <v>M</v>
       </c>
-      <c r="AU7" s="139" t="str">
+      <c r="AU7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>T</v>
       </c>
-      <c r="AV7" s="139" t="str">
+      <c r="AV7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>W</v>
       </c>
-      <c r="AW7" s="139" t="str">
+      <c r="AW7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>T</v>
       </c>
-      <c r="AX7" s="139" t="str">
+      <c r="AX7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="AY7" s="139" t="str">
+      <c r="AY7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="AZ7" s="140" t="str">
+      <c r="AZ7" s="135" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="BA7" s="138" t="str">
+      <c r="BA7" s="133" t="str">
         <f t="shared" si="3"/>
         <v>M</v>
       </c>
-      <c r="BB7" s="139" t="str">
+      <c r="BB7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>T</v>
       </c>
-      <c r="BC7" s="139" t="str">
+      <c r="BC7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>W</v>
       </c>
-      <c r="BD7" s="139" t="str">
+      <c r="BD7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>T</v>
       </c>
-      <c r="BE7" s="139" t="str">
+      <c r="BE7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="BF7" s="139" t="str">
+      <c r="BF7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="BG7" s="140" t="str">
+      <c r="BG7" s="135" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="BH7" s="138" t="str">
+      <c r="BH7" s="133" t="str">
         <f t="shared" si="3"/>
         <v>M</v>
       </c>
-      <c r="BI7" s="139" t="str">
+      <c r="BI7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>T</v>
       </c>
-      <c r="BJ7" s="139" t="str">
+      <c r="BJ7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>W</v>
       </c>
-      <c r="BK7" s="139" t="str">
+      <c r="BK7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>T</v>
       </c>
-      <c r="BL7" s="139" t="str">
+      <c r="BL7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
-      <c r="BM7" s="139" t="str">
+      <c r="BM7" s="134" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
-      <c r="BN7" s="140" t="str">
+      <c r="BN7" s="135" t="str">
         <f t="shared" si="3"/>
         <v>S</v>
       </c>
     </row>
     <row r="8" spans="1:66" s="49" customFormat="1" ht="18">
       <c r="A8" s="57"/>
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="116" t="s">
         <v>131</v>
       </c>
       <c r="C8" s="58" t="s">
@@ -4039,7 +4039,7 @@
       <c r="D8" s="59"/>
       <c r="E8" s="60"/>
       <c r="F8" s="72" t="str">
-        <f>IF(ISBLANK(E8)," - ",IF(G8=0,E8,E8+G8-1))</f>
+        <f t="shared" ref="F8:F25" si="4">IF(ISBLANK(E8)," - ",IF(G8=0,E8,E8+G8-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G8" s="61"/>
@@ -4105,27 +4105,27 @@
     </row>
     <row r="9" spans="1:66" s="55" customFormat="1" ht="18">
       <c r="A9" s="54"/>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="106" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="117" t="s">
+      <c r="C9" s="114" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="110"/>
-      <c r="E9" s="111">
+      <c r="D9" s="107"/>
+      <c r="E9" s="108">
         <v>43129</v>
       </c>
-      <c r="F9" s="112">
-        <f>IF(ISBLANK(E9)," - ",IF(G9=0,E9,E9+G9-1))</f>
+      <c r="F9" s="109">
+        <f t="shared" si="4"/>
         <v>43129</v>
       </c>
-      <c r="G9" s="113">
+      <c r="G9" s="110">
         <v>1</v>
       </c>
-      <c r="H9" s="114">
+      <c r="H9" s="111">
         <v>0</v>
       </c>
-      <c r="I9" s="115"/>
+      <c r="I9" s="112"/>
       <c r="J9" s="65"/>
       <c r="K9" s="69"/>
       <c r="L9" s="69"/>
@@ -4186,27 +4186,27 @@
     </row>
     <row r="10" spans="1:66" s="55" customFormat="1" ht="28">
       <c r="A10" s="54"/>
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="106" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="117" t="s">
+      <c r="C10" s="114" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="110"/>
-      <c r="E10" s="111">
+      <c r="D10" s="107"/>
+      <c r="E10" s="108">
         <v>43130</v>
       </c>
-      <c r="F10" s="112">
-        <f>IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+      <c r="F10" s="109">
+        <f t="shared" si="4"/>
         <v>43132</v>
       </c>
-      <c r="G10" s="113">
+      <c r="G10" s="110">
         <v>3</v>
       </c>
-      <c r="H10" s="114">
+      <c r="H10" s="111">
         <v>0</v>
       </c>
-      <c r="I10" s="115"/>
+      <c r="I10" s="112"/>
       <c r="J10" s="65"/>
       <c r="K10" s="69"/>
       <c r="L10" s="69"/>
@@ -4267,27 +4267,27 @@
     </row>
     <row r="11" spans="1:66" s="55" customFormat="1" ht="18">
       <c r="A11" s="54"/>
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="106" t="s">
         <v>133</v>
       </c>
-      <c r="C11" s="117" t="s">
+      <c r="C11" s="114" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="110"/>
-      <c r="E11" s="111">
+      <c r="D11" s="107"/>
+      <c r="E11" s="108">
         <v>43133</v>
       </c>
-      <c r="F11" s="112">
-        <f>IF(ISBLANK(E11)," - ",IF(G11=0,E11,E11+G11-1))</f>
+      <c r="F11" s="109">
+        <f t="shared" si="4"/>
         <v>43133</v>
       </c>
-      <c r="G11" s="113">
+      <c r="G11" s="110">
         <v>1</v>
       </c>
-      <c r="H11" s="114">
+      <c r="H11" s="111">
         <v>0</v>
       </c>
-      <c r="I11" s="115"/>
+      <c r="I11" s="112"/>
       <c r="J11" s="65"/>
       <c r="K11" s="69"/>
       <c r="L11" s="69"/>
@@ -4348,27 +4348,27 @@
     </row>
     <row r="12" spans="1:66" s="55" customFormat="1" ht="28">
       <c r="A12" s="54"/>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="106" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="117" t="s">
+      <c r="C12" s="114" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="110"/>
-      <c r="E12" s="111">
+      <c r="D12" s="107"/>
+      <c r="E12" s="108">
         <v>43136</v>
       </c>
-      <c r="F12" s="112">
-        <f>IF(ISBLANK(E12)," - ",IF(G12=0,E12,E12+G12-1))</f>
+      <c r="F12" s="109">
+        <f t="shared" si="4"/>
         <v>43140</v>
       </c>
-      <c r="G12" s="113">
+      <c r="G12" s="110">
         <v>5</v>
       </c>
-      <c r="H12" s="114">
+      <c r="H12" s="111">
         <v>0</v>
       </c>
-      <c r="I12" s="115"/>
+      <c r="I12" s="112"/>
       <c r="J12" s="65"/>
       <c r="K12" s="69"/>
       <c r="L12" s="69"/>
@@ -4429,7 +4429,7 @@
     </row>
     <row r="13" spans="1:66" s="49" customFormat="1" ht="18">
       <c r="A13" s="48"/>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="115" t="s">
         <v>148</v>
       </c>
       <c r="C13" s="49" t="s">
@@ -4438,7 +4438,7 @@
       <c r="D13" s="50"/>
       <c r="E13" s="67"/>
       <c r="F13" s="67" t="str">
-        <f>IF(ISBLANK(E13)," - ",IF(G13=0,E13,E13+G13-1))</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G13" s="51"/>
@@ -4503,28 +4503,28 @@
       <c r="BN13" s="71"/>
     </row>
     <row r="14" spans="1:66" s="55" customFormat="1" ht="18">
-      <c r="A14" s="116"/>
-      <c r="B14" s="108" t="s">
+      <c r="A14" s="113"/>
+      <c r="B14" s="106" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="117" t="s">
+      <c r="C14" s="114" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="110"/>
-      <c r="E14" s="111">
+      <c r="D14" s="107"/>
+      <c r="E14" s="108">
         <v>43129</v>
       </c>
-      <c r="F14" s="112">
-        <f>IF(ISBLANK(E14)," - ",IF(G14=0,E14,E14+G14-1))</f>
+      <c r="F14" s="109">
+        <f t="shared" si="4"/>
         <v>43129</v>
       </c>
-      <c r="G14" s="113">
+      <c r="G14" s="110">
         <v>1</v>
       </c>
-      <c r="H14" s="114">
+      <c r="H14" s="111">
         <v>0</v>
       </c>
-      <c r="I14" s="115"/>
+      <c r="I14" s="112"/>
       <c r="J14" s="65"/>
       <c r="K14" s="69"/>
       <c r="L14" s="69"/>
@@ -4584,28 +4584,28 @@
       <c r="BN14" s="69"/>
     </row>
     <row r="15" spans="1:66" s="55" customFormat="1" ht="56">
-      <c r="A15" s="116"/>
-      <c r="B15" s="108" t="s">
+      <c r="A15" s="113"/>
+      <c r="B15" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="117" t="s">
+      <c r="C15" s="114" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="110"/>
-      <c r="E15" s="111">
+      <c r="D15" s="107"/>
+      <c r="E15" s="108">
         <v>43130</v>
       </c>
-      <c r="F15" s="112">
-        <f>IF(ISBLANK(E15)," - ",IF(G15=0,E15,E15+G15-1))</f>
+      <c r="F15" s="109">
+        <f t="shared" si="4"/>
         <v>43133</v>
       </c>
-      <c r="G15" s="113">
+      <c r="G15" s="110">
         <v>4</v>
       </c>
-      <c r="H15" s="114">
+      <c r="H15" s="111">
         <v>0</v>
       </c>
-      <c r="I15" s="115"/>
+      <c r="I15" s="112"/>
       <c r="J15" s="65"/>
       <c r="K15" s="69"/>
       <c r="L15" s="69"/>
@@ -4665,28 +4665,28 @@
       <c r="BN15" s="69"/>
     </row>
     <row r="16" spans="1:66" s="55" customFormat="1" ht="18">
-      <c r="A16" s="116"/>
-      <c r="B16" s="108" t="s">
+      <c r="A16" s="113"/>
+      <c r="B16" s="106" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="117" t="s">
+      <c r="C16" s="114" t="s">
         <v>135</v>
       </c>
-      <c r="D16" s="110"/>
-      <c r="E16" s="111">
+      <c r="D16" s="107"/>
+      <c r="E16" s="108">
         <v>43133</v>
       </c>
-      <c r="F16" s="112">
-        <f>IF(ISBLANK(E16)," - ",IF(G16=0,E16,E16+G16-1))</f>
+      <c r="F16" s="109">
+        <f t="shared" si="4"/>
         <v>43133</v>
       </c>
-      <c r="G16" s="113">
+      <c r="G16" s="110">
         <v>1</v>
       </c>
-      <c r="H16" s="114">
+      <c r="H16" s="111">
         <v>0</v>
       </c>
-      <c r="I16" s="115"/>
+      <c r="I16" s="112"/>
       <c r="J16" s="65"/>
       <c r="K16" s="69"/>
       <c r="L16" s="69"/>
@@ -4746,28 +4746,28 @@
       <c r="BN16" s="69"/>
     </row>
     <row r="17" spans="1:66" s="55" customFormat="1" ht="42">
-      <c r="A17" s="116"/>
-      <c r="B17" s="108" t="s">
+      <c r="A17" s="113"/>
+      <c r="B17" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="117" t="s">
+      <c r="C17" s="114" t="s">
         <v>135</v>
       </c>
-      <c r="D17" s="110"/>
-      <c r="E17" s="111">
+      <c r="D17" s="107"/>
+      <c r="E17" s="108">
         <v>43136</v>
       </c>
-      <c r="F17" s="112">
-        <f>IF(ISBLANK(E17)," - ",IF(G17=0,E17,E17+G17-1))</f>
+      <c r="F17" s="109">
+        <f t="shared" si="4"/>
         <v>43140</v>
       </c>
-      <c r="G17" s="113">
+      <c r="G17" s="110">
         <v>5</v>
       </c>
-      <c r="H17" s="114">
+      <c r="H17" s="111">
         <v>0</v>
       </c>
-      <c r="I17" s="115"/>
+      <c r="I17" s="112"/>
       <c r="J17" s="65"/>
       <c r="K17" s="69"/>
       <c r="L17" s="69"/>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="18" spans="1:66" s="49" customFormat="1" ht="18">
       <c r="A18" s="48"/>
-      <c r="B18" s="118" t="s">
+      <c r="B18" s="115" t="s">
         <v>139</v>
       </c>
       <c r="C18" s="49" t="s">
@@ -4837,7 +4837,7 @@
       <c r="D18" s="50"/>
       <c r="E18" s="67"/>
       <c r="F18" s="67" t="str">
-        <f>IF(ISBLANK(E18)," - ",IF(G18=0,E18,E18+G18-1))</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G18" s="51"/>
@@ -4903,27 +4903,27 @@
     </row>
     <row r="19" spans="1:66" s="55" customFormat="1" ht="42">
       <c r="A19" s="54"/>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="117" t="s">
+      <c r="C19" s="114" t="s">
         <v>143</v>
       </c>
-      <c r="D19" s="110"/>
-      <c r="E19" s="111">
+      <c r="D19" s="107"/>
+      <c r="E19" s="108">
         <v>43143</v>
       </c>
-      <c r="F19" s="112">
-        <f>IF(ISBLANK(E19)," - ",IF(G19=0,E19,E19+G19-1))</f>
+      <c r="F19" s="109">
+        <f t="shared" si="4"/>
         <v>43145</v>
       </c>
-      <c r="G19" s="113">
+      <c r="G19" s="110">
         <v>3</v>
       </c>
-      <c r="H19" s="114">
+      <c r="H19" s="111">
         <v>0</v>
       </c>
-      <c r="I19" s="115"/>
+      <c r="I19" s="112"/>
       <c r="J19" s="65"/>
       <c r="K19" s="69"/>
       <c r="L19" s="69"/>
@@ -4984,27 +4984,27 @@
     </row>
     <row r="20" spans="1:66" s="55" customFormat="1" ht="56">
       <c r="A20" s="54"/>
-      <c r="B20" s="108" t="s">
+      <c r="B20" s="106" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="117" t="s">
+      <c r="C20" s="114" t="s">
         <v>143</v>
       </c>
-      <c r="D20" s="110"/>
-      <c r="E20" s="111">
+      <c r="D20" s="107"/>
+      <c r="E20" s="108">
         <v>43146</v>
       </c>
-      <c r="F20" s="112">
-        <f>IF(ISBLANK(E20)," - ",IF(G20=0,E20,E20+G20-1))</f>
+      <c r="F20" s="109">
+        <f t="shared" si="4"/>
         <v>43154</v>
       </c>
-      <c r="G20" s="113">
+      <c r="G20" s="110">
         <v>9</v>
       </c>
-      <c r="H20" s="114">
+      <c r="H20" s="111">
         <v>0</v>
       </c>
-      <c r="I20" s="115"/>
+      <c r="I20" s="112"/>
       <c r="J20" s="65"/>
       <c r="K20" s="69"/>
       <c r="L20" s="69"/>
@@ -5065,27 +5065,27 @@
     </row>
     <row r="21" spans="1:66" s="55" customFormat="1" ht="42">
       <c r="A21" s="54"/>
-      <c r="B21" s="108" t="s">
+      <c r="B21" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="117" t="s">
+      <c r="C21" s="114" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="110"/>
-      <c r="E21" s="111">
+      <c r="D21" s="107"/>
+      <c r="E21" s="108">
         <v>43155</v>
       </c>
-      <c r="F21" s="112">
-        <f>IF(ISBLANK(E21)," - ",IF(G21=0,E21,E21+G21-1))</f>
+      <c r="F21" s="109">
+        <f t="shared" si="4"/>
         <v>43163</v>
       </c>
-      <c r="G21" s="113">
+      <c r="G21" s="110">
         <v>9</v>
       </c>
-      <c r="H21" s="114">
+      <c r="H21" s="111">
         <v>0</v>
       </c>
-      <c r="I21" s="115"/>
+      <c r="I21" s="112"/>
       <c r="J21" s="65"/>
       <c r="K21" s="69"/>
       <c r="L21" s="69"/>
@@ -5146,7 +5146,7 @@
     </row>
     <row r="22" spans="1:66" s="49" customFormat="1" ht="18">
       <c r="A22" s="48"/>
-      <c r="B22" s="118" t="s">
+      <c r="B22" s="115" t="s">
         <v>138</v>
       </c>
       <c r="C22" s="49" t="s">
@@ -5155,7 +5155,7 @@
       <c r="D22" s="50"/>
       <c r="E22" s="67"/>
       <c r="F22" s="67" t="str">
-        <f>IF(ISBLANK(E22)," - ",IF(G22=0,E22,E22+G22-1))</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G22" s="51"/>
@@ -5221,22 +5221,24 @@
     </row>
     <row r="23" spans="1:66" s="55" customFormat="1" ht="28">
       <c r="A23" s="54"/>
-      <c r="B23" s="108" t="s">
+      <c r="B23" s="106" t="s">
         <v>144</v>
       </c>
-      <c r="C23" s="109"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="111">
+      <c r="C23" s="114" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="107"/>
+      <c r="E23" s="108">
         <v>43146</v>
       </c>
-      <c r="F23" s="112">
-        <f>IF(ISBLANK(E23)," - ",IF(G23=0,E23,E23+G23-1))</f>
+      <c r="F23" s="109">
+        <f t="shared" si="4"/>
         <v>43150</v>
       </c>
-      <c r="G23" s="113">
+      <c r="G23" s="110">
         <v>5</v>
       </c>
-      <c r="H23" s="114">
+      <c r="H23" s="111">
         <v>0</v>
       </c>
       <c r="I23" s="56"/>
@@ -5300,22 +5302,24 @@
     </row>
     <row r="24" spans="1:66" s="55" customFormat="1" ht="28">
       <c r="A24" s="54"/>
-      <c r="B24" s="108" t="s">
+      <c r="B24" s="106" t="s">
         <v>146</v>
       </c>
-      <c r="C24" s="109"/>
-      <c r="D24" s="110"/>
-      <c r="E24" s="111">
+      <c r="C24" s="114" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="107"/>
+      <c r="E24" s="108">
         <v>43151</v>
       </c>
-      <c r="F24" s="112">
-        <f>IF(ISBLANK(E24)," - ",IF(G24=0,E24,E24+G24-1))</f>
+      <c r="F24" s="109">
+        <f t="shared" si="4"/>
         <v>43160</v>
       </c>
-      <c r="G24" s="113">
+      <c r="G24" s="110">
         <v>10</v>
       </c>
-      <c r="H24" s="114">
+      <c r="H24" s="111">
         <v>0</v>
       </c>
       <c r="I24" s="56"/>
@@ -5379,22 +5383,24 @@
     </row>
     <row r="25" spans="1:66" s="55" customFormat="1" ht="28">
       <c r="A25" s="54"/>
-      <c r="B25" s="108" t="s">
+      <c r="B25" s="106" t="s">
         <v>147</v>
       </c>
-      <c r="C25" s="109"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="111">
+      <c r="C25" s="114" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="107"/>
+      <c r="E25" s="108">
         <v>43161</v>
       </c>
-      <c r="F25" s="112">
-        <f>IF(ISBLANK(E25)," - ",IF(G25=0,E25,E25+G25-1))</f>
+      <c r="F25" s="109">
+        <f t="shared" si="4"/>
         <v>43170</v>
       </c>
-      <c r="G25" s="113">
+      <c r="G25" s="110">
         <v>10</v>
       </c>
-      <c r="H25" s="114">
+      <c r="H25" s="111">
         <v>0</v>
       </c>
       <c r="I25" s="56"/>
@@ -5459,15 +5465,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -5478,6 +5475,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H25">
@@ -5806,10 +5812,10 @@
     </row>
     <row r="12" spans="1:3" s="20" customFormat="1"/>
     <row r="13" spans="1:3" ht="18">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="154" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="107"/>
+      <c r="B13" s="154"/>
     </row>
     <row r="14" spans="1:3" s="20" customFormat="1"/>
     <row r="15" spans="1:3" s="77" customFormat="1" ht="18">
@@ -5871,10 +5877,10 @@
       <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:3" s="8" customFormat="1" ht="18">
-      <c r="A24" s="107" t="s">
+      <c r="A24" s="154" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="107"/>
+      <c r="B24" s="154"/>
     </row>
     <row r="25" spans="1:3" s="8" customFormat="1" ht="45">
       <c r="A25" s="87"/>
@@ -5947,10 +5953,10 @@
       <c r="B37" s="10"/>
     </row>
     <row r="38" spans="1:2" ht="18">
-      <c r="A38" s="107" t="s">
+      <c r="A38" s="154" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="107"/>
+      <c r="B38" s="154"/>
     </row>
     <row r="39" spans="1:2" ht="30">
       <c r="B39" s="84" t="s">
@@ -5987,10 +5993,10 @@
       <c r="B48" s="11"/>
     </row>
     <row r="49" spans="1:2" ht="18">
-      <c r="A49" s="107" t="s">
+      <c r="A49" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="107"/>
+      <c r="B49" s="154"/>
     </row>
     <row r="50" spans="1:2" ht="30">
       <c r="B50" s="84" t="s">
@@ -6088,10 +6094,10 @@
       <c r="B64" s="12"/>
     </row>
     <row r="65" spans="1:2" s="20" customFormat="1" ht="18">
-      <c r="A65" s="107" t="s">
+      <c r="A65" s="154" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="107"/>
+      <c r="B65" s="154"/>
     </row>
     <row r="66" spans="1:2" s="20" customFormat="1" ht="45">
       <c r="B66" s="84" t="s">
@@ -6102,10 +6108,10 @@
       <c r="B67" s="13"/>
     </row>
     <row r="68" spans="1:2" s="8" customFormat="1" ht="18">
-      <c r="A68" s="107" t="s">
+      <c r="A68" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="107"/>
+      <c r="B68" s="154"/>
     </row>
     <row r="69" spans="1:2" s="20" customFormat="1" ht="15">
       <c r="A69" s="99" t="s">

</xml_diff>